<commit_message>
Mise en forme du tableau heure-personne
</commit_message>
<xml_diff>
--- a/docs/diagramme-de-gantt/tableau-heures-personnes.xlsx
+++ b/docs/diagramme-de-gantt/tableau-heures-personnes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ornidon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ornidon\Desktop\PDG\HEIG_VD_2016_PDG\docs\diagramme-de-gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Champion</t>
   </si>
@@ -90,14 +90,28 @@
   </si>
   <si>
     <t>Membres</t>
+  </si>
+  <si>
+    <t>Total par semaine</t>
+  </si>
+  <si>
+    <t>Total par personne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,9 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,16 +423,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.69140625" customWidth="1"/>
+    <col min="18" max="18" width="16.69140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
@@ -468,8 +487,8 @@
       <c r="Q1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" t="s">
-        <v>20</v>
+      <c r="R1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.4">
@@ -701,76 +720,85 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="B6">
+      <c r="R6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
         <f>SUM(B2:B5)</f>
         <v>17</v>
       </c>
-      <c r="C6">
-        <f t="shared" ref="C6:Q6" si="0">SUM(C2:C5)</f>
+      <c r="C7">
+        <f>SUM(C2:C5)</f>
         <v>29</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+      <c r="D7">
+        <f>SUM(D2:D5)</f>
         <v>28</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="E7">
+        <f>SUM(E2:E5)</f>
         <v>26</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
+      <c r="F7">
+        <f>SUM(F2:F5)</f>
         <v>22</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="0"/>
+      <c r="G7">
+        <f>SUM(G2:G5)</f>
         <v>26</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
+      <c r="H7">
+        <f>SUM(H2:H5)</f>
         <v>22</v>
       </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
+      <c r="I7">
+        <f>SUM(I2:I5)</f>
         <v>26</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
+      <c r="J7">
+        <f>SUM(J2:J5)</f>
         <v>26</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
+      <c r="K7">
+        <f>SUM(K2:K5)</f>
         <v>24</v>
       </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
+      <c r="L7">
+        <f>SUM(L2:L5)</f>
         <v>24</v>
       </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
+      <c r="M7">
+        <f>SUM(M2:M5)</f>
         <v>23</v>
       </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
+      <c r="N7">
+        <f>SUM(N2:N5)</f>
         <v>25</v>
       </c>
-      <c r="O6">
-        <f t="shared" si="0"/>
+      <c r="O7">
+        <f>SUM(O2:O5)</f>
         <v>24</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
+      <c r="P7">
+        <f>SUM(P2:P5)</f>
         <v>26</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="0"/>
+      <c r="Q7">
+        <f>SUM(Q2:Q5)</f>
         <v>24</v>
       </c>
-      <c r="R6">
+      <c r="R7" s="2">
         <f>SUM(R2:R5)</f>
         <v>392</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>